<commit_message>
EPBDS: replaced bean factory configuration.
</commit_message>
<xml_diff>
--- a/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/customconverters/CustomConvertersTest.xlsx
+++ b/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/customconverters/CustomConvertersTest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>classA</t>
   </si>
@@ -39,9 +39,6 @@
     <t>org.openl.rules.mapping</t>
   </si>
   <si>
-    <t>classABeanFactory</t>
-  </si>
-  <si>
     <t>Class A</t>
   </si>
   <si>
@@ -54,11 +51,6 @@
     <t>Field B</t>
   </si>
   <si>
-    <t>Class A 
-bean factory 
-class</t>
-  </si>
-  <si>
     <t>PurchaseOrderTO</t>
   </si>
   <si>
@@ -90,9 +82,6 @@
   </si>
   <si>
     <t>price</t>
-  </si>
-  <si>
-    <t>org.dozer.factory.XMLBeanFactory</t>
   </si>
   <si>
     <t>org.openl.rules.mapping.to.xmlbeans</t>
@@ -265,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -273,9 +262,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -587,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C8:I26"/>
+  <dimension ref="C8:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -599,43 +585,41 @@
     <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="3:9">
-      <c r="C8" s="7" t="s">
+    <row r="8" spans="3:8">
+      <c r="C8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="3:9">
-      <c r="C9" s="7" t="s">
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="3:8">
+      <c r="C9" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="3:9">
-      <c r="C10" s="7"/>
+    <row r="10" spans="3:8">
+      <c r="C10" s="6"/>
       <c r="D10" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="3:9">
-      <c r="C15" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="3:9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8">
+      <c r="C15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="3:8">
       <c r="C16" s="2" t="s">
         <v>0</v>
       </c>
@@ -649,202 +633,169 @@
         <v>3</v>
       </c>
       <c r="G16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8">
+      <c r="C17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8">
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8">
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8">
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8">
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8">
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8">
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8">
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8">
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8">
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="3:9" ht="45">
-      <c r="C17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="3:9">
-      <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
         <v>26</v>
-      </c>
-      <c r="F18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="3:9">
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="3:9">
-      <c r="C20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="3:9">
-      <c r="C21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="3:9">
-      <c r="C22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="3:9">
-      <c r="C23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="3:9">
-      <c r="C24" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" t="s">
-        <v>22</v>
-      </c>
-      <c r="F24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="3:9">
-      <c r="C25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="3:9">
-      <c r="C26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" t="s">
-        <v>34</v>
-      </c>
-      <c r="G26" t="s">
-        <v>24</v>
-      </c>
-      <c r="H26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I26" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C15:I15"/>
+    <mergeCell ref="C15:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -865,23 +816,23 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:3">
-      <c r="C5" s="5" t="s">
-        <v>36</v>
+      <c r="C5" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="3:3">
-      <c r="C6" s="6" t="s">
-        <v>30</v>
+      <c r="C6" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="3:3">
-      <c r="C10" s="5" t="s">
-        <v>41</v>
+      <c r="C10" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="3:3">
-      <c r="C11" s="6" t="s">
-        <v>42</v>
+      <c r="C11" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -905,11 +856,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:5">
-      <c r="C4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="C4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="3:5">
       <c r="C5" s="2" t="s">
@@ -919,29 +870,29 @@
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="3:5">
       <c r="C6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="3:5">
       <c r="C7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>